<commit_message>
covid-19 updates august 24, 2021
</commit_message>
<xml_diff>
--- a/covid.xlsx
+++ b/covid.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="10">
   <si>
     <t>Country</t>
   </si>
@@ -95,7 +95,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +105,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -121,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -129,6 +135,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,11 +411,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I506"/>
+  <dimension ref="A1:I547"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A497" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C498" sqref="C498"/>
+      <pane ySplit="1" topLeftCell="A535" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K539" sqref="K539"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -17041,6 +17048,1318 @@
         <v>738</v>
       </c>
     </row>
+    <row r="507" spans="1:9">
+      <c r="A507" t="s">
+        <v>9</v>
+      </c>
+      <c r="B507" s="1">
+        <v>44391</v>
+      </c>
+      <c r="C507">
+        <v>981392</v>
+      </c>
+      <c r="D507">
+        <v>22689</v>
+      </c>
+      <c r="E507">
+        <v>916373</v>
+      </c>
+      <c r="F507">
+        <v>42330</v>
+      </c>
+      <c r="G507" s="2">
+        <f t="shared" ref="G507:G519" si="154">C507-C506</f>
+        <v>2545</v>
+      </c>
+      <c r="H507" s="3">
+        <f t="shared" ref="H507:H519" si="155">D507-D506</f>
+        <v>47</v>
+      </c>
+      <c r="I507" s="4">
+        <f t="shared" ref="I507:I519" si="156">E507-E506</f>
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="508" spans="1:9">
+      <c r="A508" t="s">
+        <v>9</v>
+      </c>
+      <c r="B508" s="1">
+        <v>44392</v>
+      </c>
+      <c r="C508">
+        <v>983719</v>
+      </c>
+      <c r="D508">
+        <v>22720</v>
+      </c>
+      <c r="E508">
+        <v>917329</v>
+      </c>
+      <c r="F508">
+        <v>43670</v>
+      </c>
+      <c r="G508" s="2">
+        <f t="shared" si="154"/>
+        <v>2327</v>
+      </c>
+      <c r="H508" s="3">
+        <f t="shared" si="155"/>
+        <v>31</v>
+      </c>
+      <c r="I508" s="4">
+        <f t="shared" si="156"/>
+        <v>956</v>
+      </c>
+    </row>
+    <row r="509" spans="1:9">
+      <c r="A509" t="s">
+        <v>9</v>
+      </c>
+      <c r="B509" s="1">
+        <v>44393</v>
+      </c>
+      <c r="C509">
+        <v>986668</v>
+      </c>
+      <c r="D509">
+        <v>22760</v>
+      </c>
+      <c r="E509">
+        <v>918329</v>
+      </c>
+      <c r="F509">
+        <v>43670</v>
+      </c>
+      <c r="G509" s="2">
+        <f t="shared" si="154"/>
+        <v>2949</v>
+      </c>
+      <c r="H509" s="3">
+        <f t="shared" si="155"/>
+        <v>40</v>
+      </c>
+      <c r="I509" s="4">
+        <f t="shared" si="156"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="510" spans="1:9">
+      <c r="A510" t="s">
+        <v>9</v>
+      </c>
+      <c r="B510" s="1">
+        <v>44394</v>
+      </c>
+      <c r="C510">
+        <v>989275</v>
+      </c>
+      <c r="D510">
+        <v>22781</v>
+      </c>
+      <c r="E510">
+        <v>919163</v>
+      </c>
+      <c r="F510">
+        <v>47331</v>
+      </c>
+      <c r="G510" s="2">
+        <f t="shared" si="154"/>
+        <v>2607</v>
+      </c>
+      <c r="H510" s="3">
+        <f t="shared" si="155"/>
+        <v>21</v>
+      </c>
+      <c r="I510" s="4">
+        <f t="shared" si="156"/>
+        <v>834</v>
+      </c>
+    </row>
+    <row r="511" spans="1:9">
+      <c r="A511" t="s">
+        <v>9</v>
+      </c>
+      <c r="B511" s="1">
+        <v>44395</v>
+      </c>
+      <c r="C511">
+        <v>991727</v>
+      </c>
+      <c r="D511">
+        <v>22811</v>
+      </c>
+      <c r="E511">
+        <v>920066</v>
+      </c>
+      <c r="F511">
+        <v>48850</v>
+      </c>
+      <c r="G511" s="2">
+        <f t="shared" si="154"/>
+        <v>2452</v>
+      </c>
+      <c r="H511" s="3">
+        <f t="shared" si="155"/>
+        <v>30</v>
+      </c>
+      <c r="I511" s="4">
+        <f t="shared" si="156"/>
+        <v>903</v>
+      </c>
+    </row>
+    <row r="512" spans="1:9">
+      <c r="A512" t="s">
+        <v>9</v>
+      </c>
+      <c r="B512" s="1">
+        <v>44396</v>
+      </c>
+      <c r="C512">
+        <v>993872</v>
+      </c>
+      <c r="D512">
+        <v>22848</v>
+      </c>
+      <c r="E512">
+        <v>921095</v>
+      </c>
+      <c r="F512">
+        <v>48850</v>
+      </c>
+      <c r="G512" s="2">
+        <f t="shared" si="154"/>
+        <v>2145</v>
+      </c>
+      <c r="H512" s="3">
+        <f t="shared" si="155"/>
+        <v>37</v>
+      </c>
+      <c r="I512" s="4">
+        <f t="shared" si="156"/>
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="513" spans="1:9">
+      <c r="A513" t="s">
+        <v>9</v>
+      </c>
+      <c r="B513" s="1">
+        <v>44397</v>
+      </c>
+      <c r="C513">
+        <v>996451</v>
+      </c>
+      <c r="D513">
+        <v>22888</v>
+      </c>
+      <c r="E513">
+        <v>922034</v>
+      </c>
+      <c r="F513">
+        <v>51529</v>
+      </c>
+      <c r="G513" s="2">
+        <f t="shared" si="154"/>
+        <v>2579</v>
+      </c>
+      <c r="H513" s="3">
+        <f t="shared" si="155"/>
+        <v>40</v>
+      </c>
+      <c r="I513" s="4">
+        <f t="shared" si="156"/>
+        <v>939</v>
+      </c>
+    </row>
+    <row r="514" spans="1:9">
+      <c r="A514" t="s">
+        <v>9</v>
+      </c>
+      <c r="B514" s="1">
+        <v>44398</v>
+      </c>
+      <c r="C514">
+        <v>998609</v>
+      </c>
+      <c r="D514">
+        <v>22928</v>
+      </c>
+      <c r="E514">
+        <v>922929</v>
+      </c>
+      <c r="F514">
+        <v>52752</v>
+      </c>
+      <c r="G514" s="2">
+        <f t="shared" si="154"/>
+        <v>2158</v>
+      </c>
+      <c r="H514" s="3">
+        <f t="shared" si="155"/>
+        <v>40</v>
+      </c>
+      <c r="I514" s="4">
+        <f t="shared" si="156"/>
+        <v>895</v>
+      </c>
+    </row>
+    <row r="515" spans="1:9">
+      <c r="A515" t="s">
+        <v>9</v>
+      </c>
+      <c r="B515" s="1">
+        <v>44399</v>
+      </c>
+      <c r="C515">
+        <v>1000034</v>
+      </c>
+      <c r="D515">
+        <v>22939</v>
+      </c>
+      <c r="E515">
+        <v>923472</v>
+      </c>
+      <c r="F515">
+        <v>53623</v>
+      </c>
+      <c r="G515" s="2">
+        <f t="shared" si="154"/>
+        <v>1425</v>
+      </c>
+      <c r="H515" s="3">
+        <f t="shared" si="155"/>
+        <v>11</v>
+      </c>
+      <c r="I515" s="4">
+        <f t="shared" si="156"/>
+        <v>543</v>
+      </c>
+    </row>
+    <row r="516" spans="1:9">
+      <c r="A516" t="s">
+        <v>9</v>
+      </c>
+      <c r="B516" s="1">
+        <v>44400</v>
+      </c>
+      <c r="C516">
+        <v>1001875</v>
+      </c>
+      <c r="D516">
+        <v>22971</v>
+      </c>
+      <c r="E516">
+        <v>924782</v>
+      </c>
+      <c r="F516">
+        <v>54122</v>
+      </c>
+      <c r="G516" s="2">
+        <f t="shared" si="154"/>
+        <v>1841</v>
+      </c>
+      <c r="H516" s="3">
+        <f t="shared" si="155"/>
+        <v>32</v>
+      </c>
+      <c r="I516" s="4">
+        <f t="shared" si="156"/>
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="517" spans="1:9">
+      <c r="A517" t="s">
+        <v>9</v>
+      </c>
+      <c r="B517" s="1">
+        <v>44401</v>
+      </c>
+      <c r="C517">
+        <v>1004694</v>
+      </c>
+      <c r="D517">
+        <v>23016</v>
+      </c>
+      <c r="E517">
+        <v>925958</v>
+      </c>
+      <c r="F517">
+        <v>55720</v>
+      </c>
+      <c r="G517" s="2">
+        <f t="shared" si="154"/>
+        <v>2819</v>
+      </c>
+      <c r="H517" s="3">
+        <f t="shared" si="155"/>
+        <v>45</v>
+      </c>
+      <c r="I517" s="4">
+        <f t="shared" si="156"/>
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="518" spans="1:9">
+      <c r="A518" t="s">
+        <v>9</v>
+      </c>
+      <c r="B518" s="1">
+        <v>44402</v>
+      </c>
+      <c r="C518">
+        <v>1008446</v>
+      </c>
+      <c r="D518">
+        <v>23048</v>
+      </c>
+      <c r="E518">
+        <v>927599</v>
+      </c>
+      <c r="F518">
+        <v>57799</v>
+      </c>
+      <c r="G518" s="2">
+        <f t="shared" si="154"/>
+        <v>3752</v>
+      </c>
+      <c r="H518" s="3">
+        <f t="shared" si="155"/>
+        <v>32</v>
+      </c>
+      <c r="I518" s="4">
+        <f t="shared" si="156"/>
+        <v>1641</v>
+      </c>
+    </row>
+    <row r="519" spans="1:9">
+      <c r="A519" t="s">
+        <v>9</v>
+      </c>
+      <c r="B519" s="1">
+        <v>44403</v>
+      </c>
+      <c r="C519">
+        <v>1011708</v>
+      </c>
+      <c r="D519">
+        <v>23087</v>
+      </c>
+      <c r="E519">
+        <v>928722</v>
+      </c>
+      <c r="F519">
+        <v>59899</v>
+      </c>
+      <c r="G519" s="2">
+        <f t="shared" si="154"/>
+        <v>3262</v>
+      </c>
+      <c r="H519" s="3">
+        <f t="shared" si="155"/>
+        <v>39</v>
+      </c>
+      <c r="I519" s="4">
+        <f t="shared" si="156"/>
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="520" spans="1:9">
+      <c r="A520" t="s">
+        <v>9</v>
+      </c>
+      <c r="B520" s="1">
+        <v>44404</v>
+      </c>
+      <c r="C520">
+        <v>1015827</v>
+      </c>
+      <c r="D520">
+        <v>23133</v>
+      </c>
+      <c r="E520">
+        <v>935742</v>
+      </c>
+      <c r="F520">
+        <v>56952</v>
+      </c>
+      <c r="G520" s="2">
+        <f t="shared" ref="G520" si="157">C520-C519</f>
+        <v>4119</v>
+      </c>
+      <c r="H520" s="3">
+        <f t="shared" ref="H520" si="158">D520-D519</f>
+        <v>46</v>
+      </c>
+      <c r="I520" s="4">
+        <f t="shared" ref="I520" si="159">E520-E519</f>
+        <v>7020</v>
+      </c>
+    </row>
+    <row r="521" spans="1:9">
+      <c r="A521" t="s">
+        <v>9</v>
+      </c>
+      <c r="B521" s="1">
+        <v>44405</v>
+      </c>
+      <c r="C521">
+        <v>1020324</v>
+      </c>
+      <c r="D521">
+        <v>23209</v>
+      </c>
+      <c r="E521">
+        <v>937354</v>
+      </c>
+      <c r="F521">
+        <v>59761</v>
+      </c>
+      <c r="G521" s="2">
+        <f t="shared" ref="G521" si="160">C521-C520</f>
+        <v>4497</v>
+      </c>
+      <c r="H521" s="3">
+        <f t="shared" ref="H521" si="161">D521-D520</f>
+        <v>76</v>
+      </c>
+      <c r="I521" s="4">
+        <f t="shared" ref="I521" si="162">E521-E520</f>
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="522" spans="1:9">
+      <c r="A522" t="s">
+        <v>9</v>
+      </c>
+      <c r="B522" s="1">
+        <v>44406</v>
+      </c>
+      <c r="C522" s="7">
+        <v>1024861</v>
+      </c>
+      <c r="D522">
+        <v>23295</v>
+      </c>
+      <c r="E522">
+        <v>938843</v>
+      </c>
+      <c r="F522">
+        <v>62723</v>
+      </c>
+      <c r="G522" s="2">
+        <f t="shared" ref="G522:G534" si="163">C522-C521</f>
+        <v>4537</v>
+      </c>
+      <c r="H522" s="3">
+        <f t="shared" ref="H522:H534" si="164">D522-D521</f>
+        <v>86</v>
+      </c>
+      <c r="I522" s="4">
+        <f t="shared" ref="I522:I534" si="165">E522-E521</f>
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="523" spans="1:9">
+      <c r="A523" t="s">
+        <v>9</v>
+      </c>
+      <c r="B523" s="1">
+        <v>44407</v>
+      </c>
+      <c r="C523">
+        <v>1029811</v>
+      </c>
+      <c r="D523">
+        <v>23360</v>
+      </c>
+      <c r="E523">
+        <v>940164</v>
+      </c>
+      <c r="F523">
+        <v>66287</v>
+      </c>
+      <c r="G523" s="2">
+        <f t="shared" si="163"/>
+        <v>4950</v>
+      </c>
+      <c r="H523" s="3">
+        <f t="shared" si="164"/>
+        <v>65</v>
+      </c>
+      <c r="I523" s="4">
+        <f t="shared" si="165"/>
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="524" spans="1:9">
+      <c r="A524" t="s">
+        <v>9</v>
+      </c>
+      <c r="B524" s="1">
+        <v>44408</v>
+      </c>
+      <c r="C524">
+        <v>1034837</v>
+      </c>
+      <c r="D524">
+        <v>23422</v>
+      </c>
+      <c r="E524">
+        <v>941659</v>
+      </c>
+      <c r="F524">
+        <v>69756</v>
+      </c>
+      <c r="G524" s="2">
+        <f t="shared" si="163"/>
+        <v>5026</v>
+      </c>
+      <c r="H524" s="3">
+        <f t="shared" si="164"/>
+        <v>62</v>
+      </c>
+      <c r="I524" s="4">
+        <f t="shared" si="165"/>
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="525" spans="1:9">
+      <c r="A525" t="s">
+        <v>9</v>
+      </c>
+      <c r="B525" s="1">
+        <v>44409</v>
+      </c>
+      <c r="C525">
+        <v>1039695</v>
+      </c>
+      <c r="D525">
+        <v>23462</v>
+      </c>
+      <c r="E525">
+        <v>943020</v>
+      </c>
+      <c r="F525">
+        <v>73213</v>
+      </c>
+      <c r="G525" s="2">
+        <f t="shared" si="163"/>
+        <v>4858</v>
+      </c>
+      <c r="H525" s="3">
+        <f t="shared" si="164"/>
+        <v>40</v>
+      </c>
+      <c r="I525" s="4">
+        <f t="shared" si="165"/>
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="526" spans="1:9">
+      <c r="A526" t="s">
+        <v>9</v>
+      </c>
+      <c r="B526" s="1">
+        <v>44410</v>
+      </c>
+      <c r="C526">
+        <v>1043277</v>
+      </c>
+      <c r="D526">
+        <v>23529</v>
+      </c>
+      <c r="E526">
+        <v>944375</v>
+      </c>
+      <c r="F526">
+        <v>75373</v>
+      </c>
+      <c r="G526" s="2">
+        <f t="shared" si="163"/>
+        <v>3582</v>
+      </c>
+      <c r="H526" s="3">
+        <f t="shared" si="164"/>
+        <v>67</v>
+      </c>
+      <c r="I526" s="4">
+        <f t="shared" si="165"/>
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="527" spans="1:9">
+      <c r="A527" t="s">
+        <v>9</v>
+      </c>
+      <c r="B527" s="1">
+        <v>44411</v>
+      </c>
+      <c r="C527">
+        <v>1047999</v>
+      </c>
+      <c r="D527">
+        <v>23575</v>
+      </c>
+      <c r="E527">
+        <v>945829</v>
+      </c>
+      <c r="F527">
+        <v>78595</v>
+      </c>
+      <c r="G527" s="2">
+        <f t="shared" si="163"/>
+        <v>4722</v>
+      </c>
+      <c r="H527" s="3">
+        <f t="shared" si="164"/>
+        <v>46</v>
+      </c>
+      <c r="I527" s="4">
+        <f t="shared" si="165"/>
+        <v>1454</v>
+      </c>
+    </row>
+    <row r="528" spans="1:9">
+      <c r="A528" t="s">
+        <v>9</v>
+      </c>
+      <c r="B528" s="1">
+        <v>44412</v>
+      </c>
+      <c r="C528">
+        <v>1053660</v>
+      </c>
+      <c r="D528">
+        <v>23635</v>
+      </c>
+      <c r="E528">
+        <v>952616</v>
+      </c>
+      <c r="F528">
+        <v>77409</v>
+      </c>
+      <c r="G528" s="2">
+        <f t="shared" si="163"/>
+        <v>5661</v>
+      </c>
+      <c r="H528" s="3">
+        <f t="shared" si="164"/>
+        <v>60</v>
+      </c>
+      <c r="I528" s="4">
+        <f t="shared" si="165"/>
+        <v>6787</v>
+      </c>
+    </row>
+    <row r="529" spans="1:9">
+      <c r="A529" t="s">
+        <v>9</v>
+      </c>
+      <c r="B529" s="1">
+        <v>44413</v>
+      </c>
+      <c r="C529">
+        <v>1058405</v>
+      </c>
+      <c r="D529">
+        <v>23702</v>
+      </c>
+      <c r="E529">
+        <v>954711</v>
+      </c>
+      <c r="F529">
+        <v>1034703</v>
+      </c>
+      <c r="G529" s="2">
+        <f t="shared" si="163"/>
+        <v>4745</v>
+      </c>
+      <c r="H529" s="3">
+        <f t="shared" si="164"/>
+        <v>67</v>
+      </c>
+      <c r="I529" s="4">
+        <f t="shared" si="165"/>
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="530" spans="1:9">
+      <c r="A530" t="s">
+        <v>9</v>
+      </c>
+      <c r="B530" s="1">
+        <v>44414</v>
+      </c>
+      <c r="C530">
+        <v>1063125</v>
+      </c>
+      <c r="D530">
+        <v>23797</v>
+      </c>
+      <c r="E530">
+        <v>959491</v>
+      </c>
+      <c r="F530">
+        <v>1039328</v>
+      </c>
+      <c r="G530" s="2">
+        <f t="shared" si="163"/>
+        <v>4720</v>
+      </c>
+      <c r="H530" s="3">
+        <f t="shared" si="164"/>
+        <v>95</v>
+      </c>
+      <c r="I530" s="4">
+        <f t="shared" si="165"/>
+        <v>4780</v>
+      </c>
+    </row>
+    <row r="531" spans="1:9">
+      <c r="A531" t="s">
+        <v>9</v>
+      </c>
+      <c r="B531" s="1">
+        <v>44415</v>
+      </c>
+      <c r="C531">
+        <v>1067580</v>
+      </c>
+      <c r="D531">
+        <v>23865</v>
+      </c>
+      <c r="E531">
+        <v>961639</v>
+      </c>
+      <c r="F531">
+        <v>1043715</v>
+      </c>
+      <c r="G531" s="2">
+        <f t="shared" si="163"/>
+        <v>4455</v>
+      </c>
+      <c r="H531" s="3">
+        <f t="shared" si="164"/>
+        <v>68</v>
+      </c>
+      <c r="I531" s="4">
+        <f t="shared" si="165"/>
+        <v>2148</v>
+      </c>
+    </row>
+    <row r="532" spans="1:9">
+      <c r="A532" t="s">
+        <v>9</v>
+      </c>
+      <c r="B532" s="1">
+        <v>44416</v>
+      </c>
+      <c r="C532">
+        <v>1071620</v>
+      </c>
+      <c r="D532">
+        <v>23918</v>
+      </c>
+      <c r="E532">
+        <v>964404</v>
+      </c>
+      <c r="F532">
+        <v>1047702</v>
+      </c>
+      <c r="G532" s="2">
+        <f t="shared" si="163"/>
+        <v>4040</v>
+      </c>
+      <c r="H532" s="3">
+        <f t="shared" si="164"/>
+        <v>53</v>
+      </c>
+      <c r="I532" s="4">
+        <f t="shared" si="165"/>
+        <v>2765</v>
+      </c>
+    </row>
+    <row r="533" spans="1:9">
+      <c r="A533" t="s">
+        <v>9</v>
+      </c>
+      <c r="B533" s="1">
+        <v>44417</v>
+      </c>
+      <c r="C533">
+        <v>1075504</v>
+      </c>
+      <c r="D533">
+        <v>24004</v>
+      </c>
+      <c r="E533">
+        <v>967073</v>
+      </c>
+      <c r="F533">
+        <v>1051500</v>
+      </c>
+      <c r="G533" s="2">
+        <f t="shared" si="163"/>
+        <v>3884</v>
+      </c>
+      <c r="H533" s="3">
+        <f t="shared" si="164"/>
+        <v>86</v>
+      </c>
+      <c r="I533" s="4">
+        <f t="shared" si="165"/>
+        <v>2669</v>
+      </c>
+    </row>
+    <row r="534" spans="1:9">
+      <c r="A534" t="s">
+        <v>9</v>
+      </c>
+      <c r="B534" s="1">
+        <v>44418</v>
+      </c>
+      <c r="C534">
+        <v>1080360</v>
+      </c>
+      <c r="D534">
+        <v>24085</v>
+      </c>
+      <c r="E534">
+        <v>972098</v>
+      </c>
+      <c r="F534">
+        <v>1056275</v>
+      </c>
+      <c r="G534" s="2">
+        <f t="shared" si="163"/>
+        <v>4856</v>
+      </c>
+      <c r="H534" s="3">
+        <f t="shared" si="164"/>
+        <v>81</v>
+      </c>
+      <c r="I534" s="4">
+        <f t="shared" si="165"/>
+        <v>5025</v>
+      </c>
+    </row>
+    <row r="535" spans="1:9">
+      <c r="A535" t="s">
+        <v>9</v>
+      </c>
+      <c r="B535" s="1">
+        <v>44419</v>
+      </c>
+      <c r="C535" s="7">
+        <v>1085294</v>
+      </c>
+      <c r="D535">
+        <v>24187</v>
+      </c>
+      <c r="E535">
+        <v>975474</v>
+      </c>
+      <c r="F535">
+        <v>1061107</v>
+      </c>
+      <c r="G535" s="2">
+        <f t="shared" ref="G535:G547" si="166">C535-C534</f>
+        <v>4934</v>
+      </c>
+      <c r="H535" s="3">
+        <f t="shared" ref="H535:H547" si="167">D535-D534</f>
+        <v>102</v>
+      </c>
+      <c r="I535" s="4">
+        <f t="shared" ref="I535:I547" si="168">E535-E534</f>
+        <v>3376</v>
+      </c>
+    </row>
+    <row r="536" spans="1:9">
+      <c r="A536" t="s">
+        <v>9</v>
+      </c>
+      <c r="B536" s="1">
+        <v>44420</v>
+      </c>
+      <c r="C536">
+        <v>1089913</v>
+      </c>
+      <c r="D536">
+        <v>24266</v>
+      </c>
+      <c r="E536">
+        <v>979411</v>
+      </c>
+      <c r="F536">
+        <v>1065647</v>
+      </c>
+      <c r="G536" s="2">
+        <f t="shared" si="166"/>
+        <v>4619</v>
+      </c>
+      <c r="H536" s="3">
+        <f t="shared" si="167"/>
+        <v>79</v>
+      </c>
+      <c r="I536" s="4">
+        <f t="shared" si="168"/>
+        <v>3937</v>
+      </c>
+    </row>
+    <row r="537" spans="1:9">
+      <c r="A537" t="s">
+        <v>9</v>
+      </c>
+      <c r="B537" s="1">
+        <v>44421</v>
+      </c>
+      <c r="C537">
+        <v>1094699</v>
+      </c>
+      <c r="D537">
+        <v>24339</v>
+      </c>
+      <c r="E537">
+        <v>983754</v>
+      </c>
+      <c r="F537">
+        <v>1070360</v>
+      </c>
+      <c r="G537" s="2">
+        <f t="shared" si="166"/>
+        <v>4786</v>
+      </c>
+      <c r="H537" s="3">
+        <f t="shared" si="167"/>
+        <v>73</v>
+      </c>
+      <c r="I537" s="4">
+        <f t="shared" si="168"/>
+        <v>4343</v>
+      </c>
+    </row>
+    <row r="538" spans="1:9">
+      <c r="A538" t="s">
+        <v>9</v>
+      </c>
+      <c r="B538" s="1">
+        <v>44422</v>
+      </c>
+      <c r="C538">
+        <v>1098410</v>
+      </c>
+      <c r="D538">
+        <v>24406</v>
+      </c>
+      <c r="E538">
+        <v>986795</v>
+      </c>
+      <c r="F538">
+        <v>1070360</v>
+      </c>
+      <c r="G538" s="2">
+        <f t="shared" si="166"/>
+        <v>3711</v>
+      </c>
+      <c r="H538" s="3">
+        <f t="shared" si="167"/>
+        <v>67</v>
+      </c>
+      <c r="I538" s="4">
+        <f t="shared" si="168"/>
+        <v>3041</v>
+      </c>
+    </row>
+    <row r="539" spans="1:9">
+      <c r="A539" t="s">
+        <v>9</v>
+      </c>
+      <c r="B539" s="1">
+        <v>44423</v>
+      </c>
+      <c r="C539">
+        <v>1102079</v>
+      </c>
+      <c r="D539">
+        <v>24478</v>
+      </c>
+      <c r="E539">
+        <v>989013</v>
+      </c>
+      <c r="F539">
+        <v>1077601</v>
+      </c>
+      <c r="G539" s="2">
+        <f t="shared" si="166"/>
+        <v>3669</v>
+      </c>
+      <c r="H539" s="3">
+        <f t="shared" si="167"/>
+        <v>72</v>
+      </c>
+      <c r="I539" s="4">
+        <f t="shared" si="168"/>
+        <v>2218</v>
+      </c>
+    </row>
+    <row r="540" spans="1:9">
+      <c r="A540" t="s">
+        <v>9</v>
+      </c>
+      <c r="B540" s="1">
+        <v>44424</v>
+      </c>
+      <c r="C540">
+        <v>1105300</v>
+      </c>
+      <c r="D540">
+        <v>24573</v>
+      </c>
+      <c r="E540">
+        <v>993304</v>
+      </c>
+      <c r="F540">
+        <v>1080727</v>
+      </c>
+      <c r="G540" s="2">
+        <f t="shared" si="166"/>
+        <v>3221</v>
+      </c>
+      <c r="H540" s="3">
+        <f t="shared" si="167"/>
+        <v>95</v>
+      </c>
+      <c r="I540" s="4">
+        <f t="shared" si="168"/>
+        <v>4291</v>
+      </c>
+    </row>
+    <row r="541" spans="1:9">
+      <c r="A541" t="s">
+        <v>9</v>
+      </c>
+      <c r="B541" s="1">
+        <v>44425</v>
+      </c>
+      <c r="C541">
+        <v>1109274</v>
+      </c>
+      <c r="D541">
+        <v>24639</v>
+      </c>
+      <c r="E541">
+        <v>996426</v>
+      </c>
+      <c r="F541">
+        <v>1080727</v>
+      </c>
+      <c r="G541" s="2">
+        <f t="shared" si="166"/>
+        <v>3974</v>
+      </c>
+      <c r="H541" s="3">
+        <f t="shared" si="167"/>
+        <v>66</v>
+      </c>
+      <c r="I541" s="4">
+        <f t="shared" si="168"/>
+        <v>3122</v>
+      </c>
+    </row>
+    <row r="542" spans="1:9">
+      <c r="A542" t="s">
+        <v>9</v>
+      </c>
+      <c r="B542" s="1">
+        <v>44426</v>
+      </c>
+      <c r="C542">
+        <v>1113647</v>
+      </c>
+      <c r="D542">
+        <v>24713</v>
+      </c>
+      <c r="E542">
+        <v>999403</v>
+      </c>
+      <c r="F542">
+        <v>1084635</v>
+      </c>
+      <c r="G542" s="2">
+        <f t="shared" si="166"/>
+        <v>4373</v>
+      </c>
+      <c r="H542" s="3">
+        <f t="shared" si="167"/>
+        <v>74</v>
+      </c>
+      <c r="I542" s="4">
+        <f t="shared" si="168"/>
+        <v>2977</v>
+      </c>
+    </row>
+    <row r="543" spans="1:9">
+      <c r="A543" t="s">
+        <v>9</v>
+      </c>
+      <c r="B543" s="1">
+        <v>44427</v>
+      </c>
+      <c r="C543">
+        <v>1116886</v>
+      </c>
+      <c r="D543">
+        <v>24783</v>
+      </c>
+      <c r="E543">
+        <v>1002430</v>
+      </c>
+      <c r="F543">
+        <v>1092103</v>
+      </c>
+      <c r="G543" s="2">
+        <f t="shared" si="166"/>
+        <v>3239</v>
+      </c>
+      <c r="H543" s="3">
+        <f t="shared" si="167"/>
+        <v>70</v>
+      </c>
+      <c r="I543" s="4">
+        <f t="shared" si="168"/>
+        <v>3027</v>
+      </c>
+    </row>
+    <row r="544" spans="1:9">
+      <c r="A544" t="s">
+        <v>9</v>
+      </c>
+      <c r="B544" s="1">
+        <v>44428</v>
+      </c>
+      <c r="C544">
+        <v>1119970</v>
+      </c>
+      <c r="D544">
+        <v>24848</v>
+      </c>
+      <c r="E544">
+        <v>1006078</v>
+      </c>
+      <c r="F544">
+        <v>1095122</v>
+      </c>
+      <c r="G544" s="2">
+        <f t="shared" si="166"/>
+        <v>3084</v>
+      </c>
+      <c r="H544" s="3">
+        <f t="shared" si="167"/>
+        <v>65</v>
+      </c>
+      <c r="I544" s="4">
+        <f t="shared" si="168"/>
+        <v>3648</v>
+      </c>
+    </row>
+    <row r="545" spans="1:9">
+      <c r="A545" t="s">
+        <v>9</v>
+      </c>
+      <c r="B545" s="1">
+        <v>44429</v>
+      </c>
+      <c r="C545">
+        <v>1123812</v>
+      </c>
+      <c r="D545">
+        <v>24923</v>
+      </c>
+      <c r="E545">
+        <v>1009555</v>
+      </c>
+      <c r="F545">
+        <v>1098889</v>
+      </c>
+      <c r="G545" s="2">
+        <f t="shared" si="166"/>
+        <v>3842</v>
+      </c>
+      <c r="H545" s="3">
+        <f t="shared" si="167"/>
+        <v>75</v>
+      </c>
+      <c r="I545" s="4">
+        <f t="shared" si="168"/>
+        <v>3477</v>
+      </c>
+    </row>
+    <row r="546" spans="1:9">
+      <c r="A546" t="s">
+        <v>9</v>
+      </c>
+      <c r="B546" s="1">
+        <v>44430</v>
+      </c>
+      <c r="C546">
+        <v>1127584</v>
+      </c>
+      <c r="D546">
+        <v>25003</v>
+      </c>
+      <c r="E546">
+        <v>1012662</v>
+      </c>
+      <c r="F546">
+        <v>1102581</v>
+      </c>
+      <c r="G546" s="2">
+        <f t="shared" si="166"/>
+        <v>3772</v>
+      </c>
+      <c r="H546" s="3">
+        <f t="shared" si="167"/>
+        <v>80</v>
+      </c>
+      <c r="I546" s="4">
+        <f t="shared" si="168"/>
+        <v>3107</v>
+      </c>
+    </row>
+    <row r="547" spans="1:9">
+      <c r="A547" t="s">
+        <v>9</v>
+      </c>
+      <c r="B547" s="1">
+        <v>44431</v>
+      </c>
+      <c r="C547">
+        <v>1131659</v>
+      </c>
+      <c r="D547">
+        <v>25094</v>
+      </c>
+      <c r="E547">
+        <v>1015519</v>
+      </c>
+      <c r="F547">
+        <v>1106565</v>
+      </c>
+      <c r="G547" s="2">
+        <f t="shared" si="166"/>
+        <v>4075</v>
+      </c>
+      <c r="H547" s="3">
+        <f t="shared" si="167"/>
+        <v>91</v>
+      </c>
+      <c r="I547" s="4">
+        <f t="shared" si="168"/>
+        <v>2857</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>